<commit_message>
partie annalyse rempli à peu près lol
</commit_message>
<xml_diff>
--- a/Planificateur de projet Gantt1.xlsx
+++ b/Planificateur de projet Gantt1.xlsx
@@ -20,7 +20,11 @@
     <definedName name="PourcentageAchevéAprès">(projet!A$8=MEDIAN(projet!A$8,projet!$E1,projet!$E1+projet!$F1)*(projet!$E1&gt;0))*((projet!A$8&lt;(INT(projet!$E1+projet!$F1*projet!$G1)))+(projet!A$8=projet!$E1))*(projet!$G1&gt;0)</definedName>
   </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -151,9 +155,6 @@
     <t>ACHEVÉ</t>
   </si>
   <si>
-    <t>PÉRIODES</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -190,36 +191,6 @@
     </r>
   </si>
   <si>
-    <t>Activité 01</t>
-  </si>
-  <si>
-    <t>Activité 02</t>
-  </si>
-  <si>
-    <t>Activité 03</t>
-  </si>
-  <si>
-    <t>Activité 04</t>
-  </si>
-  <si>
-    <t>Activité 05</t>
-  </si>
-  <si>
-    <t>Activité 06</t>
-  </si>
-  <si>
-    <t>Activité 07</t>
-  </si>
-  <si>
-    <t>Activité 08</t>
-  </si>
-  <si>
-    <t>Activité 09</t>
-  </si>
-  <si>
-    <t>Activité 10</t>
-  </si>
-  <si>
     <t>Activité 11</t>
   </si>
   <si>
@@ -269,13 +240,46 @@
   </si>
   <si>
     <t>Projet CPOA - GPTL</t>
+  </si>
+  <si>
+    <t>Planification</t>
+  </si>
+  <si>
+    <t>Hébergement</t>
+  </si>
+  <si>
+    <t>Diagramme de classe hébergement</t>
+  </si>
+  <si>
+    <t>Diagramme de séquence hébergement</t>
+  </si>
+  <si>
+    <t>Cas d'utilisation hébergement</t>
+  </si>
+  <si>
+    <t>Séance</t>
+  </si>
+  <si>
+    <t>Planning des matchs</t>
+  </si>
+  <si>
+    <t>Analyse</t>
+  </si>
+  <si>
+    <t>Diagramme de classe planning</t>
+  </si>
+  <si>
+    <t>Diagramme de séquence planning</t>
+  </si>
+  <si>
+    <t>Cas d'utilisation planning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -401,8 +405,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,6 +428,12 @@
       <patternFill patternType="lightUp">
         <fgColor theme="7"/>
         <bgColor theme="7" tint="0.59996337778862885"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
@@ -440,7 +456,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,11 +537,11 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -538,10 +566,10 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="6">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="7">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="7">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="7" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="7" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -556,12 +584,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -574,13 +608,19 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -594,7 +634,150 @@
     <cellStyle name="Project Headers" xfId="4"/>
     <cellStyle name="Titre 1" xfId="1" builtinId="16" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="7"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -617,7 +800,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="période_sélectionnée" max="60" min="1" page="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="période_sélectionnée" max="60" min="1" page="10" val="8"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -902,16 +1085,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:BQ34"/>
+  <dimension ref="A2:BQ33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB22" sqref="AB22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.58203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.08203125" style="2" customWidth="1"/>
     <col min="3" max="5" width="7.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="24.58203125" style="7" customWidth="1"/>
@@ -920,9 +1103,9 @@
     <col min="29" max="70" width="4.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:69" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="21" t="s">
-        <v>40</v>
+    <row r="2" spans="1:69" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="23" t="s">
+        <v>29</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -930,7 +1113,7 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="2:69" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:69" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -945,22 +1128,22 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
-      <c r="R3" s="16" t="s">
+      <c r="R3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="T3" s="11"/>
-      <c r="U3" s="16" t="s">
+      <c r="U3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="X3" s="20"/>
+      <c r="X3" s="12"/>
       <c r="Y3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AC3" s="12"/>
+      <c r="AC3" s="13"/>
       <c r="AD3" s="6" t="s">
         <v>0</v>
       </c>
@@ -968,12 +1151,12 @@
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
-      <c r="AK3" s="13"/>
+      <c r="AK3" s="14"/>
       <c r="AL3" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -986,27 +1169,27 @@
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
     </row>
-    <row r="5" spans="2:69" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.4">
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
     </row>
-    <row r="6" spans="2:69" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:69" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="F6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="G6" s="19" t="s">
         <v>12</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>13</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1015,7 +1198,7 @@
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
     </row>
-    <row r="7" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1036,12 +1219,12 @@
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="18"/>
+    <row r="8" spans="1:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="20"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1230,530 +1413,558 @@
       </c>
       <c r="BQ8" s="1"/>
     </row>
-    <row r="9" spans="2:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="19" t="s">
+    <row r="9" spans="1:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="15">
+        <v>1</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15">
+        <v>2</v>
+      </c>
+      <c r="G9" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="24"/>
+      <c r="B10" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="15">
+        <v>4</v>
+      </c>
+      <c r="D10" s="15">
+        <v>15</v>
+      </c>
+      <c r="E10" s="15">
+        <v>4</v>
+      </c>
+      <c r="F10" s="15">
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="24"/>
+      <c r="B11" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="15">
+        <v>4</v>
+      </c>
+      <c r="D11" s="15">
+        <v>2</v>
+      </c>
+      <c r="E11" s="15">
+        <v>4</v>
+      </c>
+      <c r="F11" s="15">
+        <v>2</v>
+      </c>
+      <c r="G11" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="24"/>
+      <c r="B12" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="15">
+        <v>6</v>
+      </c>
+      <c r="D12" s="15">
+        <v>2</v>
+      </c>
+      <c r="E12" s="15">
+        <v>6</v>
+      </c>
+      <c r="F12" s="15">
+        <v>1</v>
+      </c>
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="24"/>
+      <c r="B13" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="15">
+        <v>7</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1</v>
+      </c>
+      <c r="E13" s="15">
+        <v>4</v>
+      </c>
+      <c r="F13" s="15">
+        <v>2</v>
+      </c>
+      <c r="G13" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="24"/>
+      <c r="B14" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="15">
+        <v>5</v>
+      </c>
+      <c r="D14" s="15">
+        <v>3</v>
+      </c>
+      <c r="E14" s="15">
+        <v>5</v>
+      </c>
+      <c r="F14" s="15">
+        <v>0</v>
+      </c>
+      <c r="G14" s="16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="24"/>
+      <c r="B15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="15">
+        <v>5</v>
+      </c>
+      <c r="D15" s="15">
+        <v>2</v>
+      </c>
+      <c r="E15" s="15">
+        <v>5</v>
+      </c>
+      <c r="F15" s="15">
+        <v>2</v>
+      </c>
+      <c r="G15" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="24"/>
+      <c r="B16" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="15">
+        <v>5</v>
+      </c>
+      <c r="D16" s="15">
+        <v>2</v>
+      </c>
+      <c r="E16" s="15">
+        <v>5</v>
+      </c>
+      <c r="F16" s="15">
+        <v>2</v>
+      </c>
+      <c r="G16" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="24"/>
+      <c r="B17" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="15">
+        <v>7</v>
+      </c>
+      <c r="D17" s="15">
+        <v>1</v>
+      </c>
+      <c r="E17" s="15">
+        <v>7</v>
+      </c>
+      <c r="F17" s="15">
+        <v>1</v>
+      </c>
+      <c r="G17" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="17">
+        <v>0</v>
+      </c>
+      <c r="D18" s="15">
+        <v>0</v>
+      </c>
+      <c r="E18" s="15">
+        <v>0</v>
+      </c>
+      <c r="F18" s="15">
+        <v>0</v>
+      </c>
+      <c r="G18" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C19" s="15">
+        <v>9</v>
+      </c>
+      <c r="D19" s="15">
+        <v>3</v>
+      </c>
+      <c r="E19" s="15">
+        <v>9</v>
+      </c>
+      <c r="F19" s="15">
+        <v>3</v>
+      </c>
+      <c r="G19" s="16">
         <v>0</v>
       </c>
-      <c r="D9" s="14">
+    </row>
+    <row r="20" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="15">
+        <v>9</v>
+      </c>
+      <c r="D20" s="15">
+        <v>6</v>
+      </c>
+      <c r="E20" s="15">
+        <v>9</v>
+      </c>
+      <c r="F20" s="15">
+        <v>7</v>
+      </c>
+      <c r="G20" s="16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="15">
+        <v>9</v>
+      </c>
+      <c r="D21" s="15">
+        <v>3</v>
+      </c>
+      <c r="E21" s="15">
+        <v>9</v>
+      </c>
+      <c r="F21" s="15">
+        <v>1</v>
+      </c>
+      <c r="G21" s="16">
         <v>0</v>
       </c>
-      <c r="E9" s="14">
+    </row>
+    <row r="22" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="15">
+        <v>9</v>
+      </c>
+      <c r="D22" s="15">
+        <v>4</v>
+      </c>
+      <c r="E22" s="15">
+        <v>8</v>
+      </c>
+      <c r="F22" s="15">
+        <v>5</v>
+      </c>
+      <c r="G22" s="16">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="15">
+        <v>10</v>
+      </c>
+      <c r="D23" s="15">
+        <v>5</v>
+      </c>
+      <c r="E23" s="15">
+        <v>10</v>
+      </c>
+      <c r="F23" s="15">
+        <v>3</v>
+      </c>
+      <c r="G23" s="16">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="15">
+        <v>11</v>
+      </c>
+      <c r="D24" s="15">
+        <v>2</v>
+      </c>
+      <c r="E24" s="15">
+        <v>11</v>
+      </c>
+      <c r="F24" s="15">
+        <v>5</v>
+      </c>
+      <c r="G24" s="16">
         <v>0</v>
       </c>
-      <c r="F9" s="14">
+    </row>
+    <row r="25" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="15">
+        <v>12</v>
+      </c>
+      <c r="D25" s="15">
+        <v>6</v>
+      </c>
+      <c r="E25" s="15">
+        <v>12</v>
+      </c>
+      <c r="F25" s="15">
+        <v>7</v>
+      </c>
+      <c r="G25" s="16">
         <v>0</v>
       </c>
-      <c r="G9" s="15">
+    </row>
+    <row r="26" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="15">
+        <v>12</v>
+      </c>
+      <c r="D26" s="15">
+        <v>1</v>
+      </c>
+      <c r="E26" s="15">
+        <v>12</v>
+      </c>
+      <c r="F26" s="15">
+        <v>5</v>
+      </c>
+      <c r="G26" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="19" t="s">
+    <row r="27" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="15">
+        <v>14</v>
+      </c>
+      <c r="D27" s="15">
+        <v>5</v>
+      </c>
+      <c r="E27" s="15">
+        <v>14</v>
+      </c>
+      <c r="F27" s="15">
+        <v>6</v>
+      </c>
+      <c r="G27" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="15">
+        <v>14</v>
+      </c>
+      <c r="D28" s="15">
+        <v>8</v>
+      </c>
+      <c r="E28" s="15">
+        <v>14</v>
+      </c>
+      <c r="F28" s="15">
+        <v>2</v>
+      </c>
+      <c r="G28" s="16">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="15">
+        <v>14</v>
+      </c>
+      <c r="D29" s="15">
+        <v>7</v>
+      </c>
+      <c r="E29" s="15">
+        <v>14</v>
+      </c>
+      <c r="F29" s="15">
+        <v>3</v>
+      </c>
+      <c r="G29" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="15">
         <v>15</v>
       </c>
-      <c r="C10" s="14">
+      <c r="D30" s="15">
+        <v>4</v>
+      </c>
+      <c r="E30" s="15">
+        <v>15</v>
+      </c>
+      <c r="F30" s="15">
+        <v>8</v>
+      </c>
+      <c r="G30" s="16">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="15">
+        <v>15</v>
+      </c>
+      <c r="D31" s="15">
+        <v>5</v>
+      </c>
+      <c r="E31" s="15">
+        <v>15</v>
+      </c>
+      <c r="F31" s="15">
+        <v>3</v>
+      </c>
+      <c r="G31" s="16">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="15">
+        <v>15</v>
+      </c>
+      <c r="D32" s="15">
+        <v>8</v>
+      </c>
+      <c r="E32" s="15">
+        <v>15</v>
+      </c>
+      <c r="F32" s="15">
+        <v>5</v>
+      </c>
+      <c r="G32" s="16">
         <v>0</v>
       </c>
-      <c r="D10" s="14">
-        <v>0</v>
-      </c>
-      <c r="E10" s="14">
-        <v>0</v>
-      </c>
-      <c r="F10" s="14">
-        <v>0</v>
-      </c>
-      <c r="G10" s="15">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="19" t="s">
+    </row>
+    <row r="33" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="15">
         <v>16</v>
       </c>
-      <c r="C11" s="14">
-        <v>0</v>
-      </c>
-      <c r="D11" s="14">
-        <v>0</v>
-      </c>
-      <c r="E11" s="14">
-        <v>0</v>
-      </c>
-      <c r="F11" s="14">
-        <v>0</v>
-      </c>
-      <c r="G11" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="14">
-        <v>0</v>
-      </c>
-      <c r="D12" s="14">
-        <v>0</v>
-      </c>
-      <c r="E12" s="14">
-        <v>0</v>
-      </c>
-      <c r="F12" s="14">
-        <v>0</v>
-      </c>
-      <c r="G12" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="14">
-        <v>0</v>
-      </c>
-      <c r="D13" s="14">
-        <v>0</v>
-      </c>
-      <c r="E13" s="14">
-        <v>0</v>
-      </c>
-      <c r="F13" s="14">
-        <v>0</v>
-      </c>
-      <c r="G13" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="14">
-        <v>0</v>
-      </c>
-      <c r="D14" s="14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="14">
-        <v>0</v>
-      </c>
-      <c r="D15" s="14">
-        <v>0</v>
-      </c>
-      <c r="E15" s="14">
-        <v>0</v>
-      </c>
-      <c r="F15" s="14">
-        <v>0</v>
-      </c>
-      <c r="G15" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:69" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="14">
-        <v>0</v>
-      </c>
-      <c r="D16" s="14">
-        <v>0</v>
-      </c>
-      <c r="E16" s="14">
-        <v>0</v>
-      </c>
-      <c r="F16" s="14">
-        <v>0</v>
-      </c>
-      <c r="G16" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="14">
-        <v>0</v>
-      </c>
-      <c r="D17" s="14">
-        <v>0</v>
-      </c>
-      <c r="E17" s="14">
-        <v>0</v>
-      </c>
-      <c r="F17" s="14">
-        <v>0</v>
-      </c>
-      <c r="G17" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="14">
-        <v>0</v>
-      </c>
-      <c r="D18" s="14">
-        <v>0</v>
-      </c>
-      <c r="E18" s="14">
-        <v>0</v>
-      </c>
-      <c r="F18" s="14">
-        <v>0</v>
-      </c>
-      <c r="G18" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="14">
-        <v>0</v>
-      </c>
-      <c r="D19" s="14">
-        <v>0</v>
-      </c>
-      <c r="E19" s="14">
-        <v>0</v>
-      </c>
-      <c r="F19" s="14">
-        <v>0</v>
-      </c>
-      <c r="G19" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="14">
-        <v>0</v>
-      </c>
-      <c r="D20" s="14">
-        <v>0</v>
-      </c>
-      <c r="E20" s="14">
-        <v>0</v>
-      </c>
-      <c r="F20" s="14">
-        <v>0</v>
-      </c>
-      <c r="G20" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="14">
-        <v>0</v>
-      </c>
-      <c r="D21" s="14">
-        <v>0</v>
-      </c>
-      <c r="E21" s="14">
-        <v>0</v>
-      </c>
-      <c r="F21" s="14">
-        <v>0</v>
-      </c>
-      <c r="G21" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="14">
-        <v>0</v>
-      </c>
-      <c r="D22" s="14">
-        <v>0</v>
-      </c>
-      <c r="E22" s="14">
-        <v>0</v>
-      </c>
-      <c r="F22" s="14">
-        <v>0</v>
-      </c>
-      <c r="G22" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="19" t="s">
+      <c r="D33" s="15">
         <v>28</v>
       </c>
-      <c r="C23" s="14">
-        <v>0</v>
-      </c>
-      <c r="D23" s="14">
-        <v>0</v>
-      </c>
-      <c r="E23" s="14">
-        <v>0</v>
-      </c>
-      <c r="F23" s="14">
-        <v>0</v>
-      </c>
-      <c r="G23" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="14">
-        <v>0</v>
-      </c>
-      <c r="D24" s="14">
-        <v>0</v>
-      </c>
-      <c r="E24" s="14">
-        <v>0</v>
-      </c>
-      <c r="F24" s="14">
-        <v>0</v>
-      </c>
-      <c r="G24" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="19" t="s">
+      <c r="E33" s="15">
+        <v>16</v>
+      </c>
+      <c r="F33" s="15">
         <v>30</v>
       </c>
-      <c r="C25" s="14">
-        <v>0</v>
-      </c>
-      <c r="D25" s="14">
-        <v>0</v>
-      </c>
-      <c r="E25" s="14">
-        <v>0</v>
-      </c>
-      <c r="F25" s="14">
-        <v>0</v>
-      </c>
-      <c r="G25" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="14">
-        <v>0</v>
-      </c>
-      <c r="D26" s="14">
-        <v>0</v>
-      </c>
-      <c r="E26" s="14">
-        <v>0</v>
-      </c>
-      <c r="F26" s="14">
-        <v>0</v>
-      </c>
-      <c r="G26" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="14">
-        <v>0</v>
-      </c>
-      <c r="D27" s="14">
-        <v>0</v>
-      </c>
-      <c r="E27" s="14">
-        <v>0</v>
-      </c>
-      <c r="F27" s="14">
-        <v>0</v>
-      </c>
-      <c r="G27" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="14">
-        <v>0</v>
-      </c>
-      <c r="D28" s="14">
-        <v>0</v>
-      </c>
-      <c r="E28" s="14">
-        <v>0</v>
-      </c>
-      <c r="F28" s="14">
-        <v>0</v>
-      </c>
-      <c r="G28" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="14">
-        <v>0</v>
-      </c>
-      <c r="D29" s="14">
-        <v>0</v>
-      </c>
-      <c r="E29" s="14">
-        <v>0</v>
-      </c>
-      <c r="F29" s="14">
-        <v>0</v>
-      </c>
-      <c r="G29" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="14">
-        <v>0</v>
-      </c>
-      <c r="D30" s="14">
-        <v>0</v>
-      </c>
-      <c r="E30" s="14">
-        <v>0</v>
-      </c>
-      <c r="F30" s="14">
-        <v>0</v>
-      </c>
-      <c r="G30" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="14">
-        <v>0</v>
-      </c>
-      <c r="D31" s="14">
-        <v>0</v>
-      </c>
-      <c r="E31" s="14">
-        <v>0</v>
-      </c>
-      <c r="F31" s="14">
-        <v>0</v>
-      </c>
-      <c r="G31" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="14">
-        <v>0</v>
-      </c>
-      <c r="D32" s="14">
-        <v>0</v>
-      </c>
-      <c r="E32" s="14">
-        <v>0</v>
-      </c>
-      <c r="F32" s="14">
-        <v>0</v>
-      </c>
-      <c r="G32" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="14">
-        <v>0</v>
-      </c>
-      <c r="D33" s="14">
-        <v>0</v>
-      </c>
-      <c r="E33" s="14">
-        <v>0</v>
-      </c>
-      <c r="F33" s="14">
-        <v>0</v>
-      </c>
-      <c r="G33" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="14">
-        <v>0</v>
-      </c>
-      <c r="D34" s="14">
-        <v>0</v>
-      </c>
-      <c r="E34" s="14">
-        <v>0</v>
-      </c>
-      <c r="F34" s="14">
-        <v>0</v>
-      </c>
-      <c r="G34" s="15">
-        <v>0</v>
+      <c r="G33" s="16">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:G4"/>
+    <mergeCell ref="A9:A17"/>
   </mergeCells>
+  <conditionalFormatting sqref="I9:BP33">
+    <cfRule type="expression" dxfId="9" priority="1">
+      <formula>PourcentageAchevé</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="3">
+      <formula>PourcentageAchevéAprès</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="4">
+      <formula>Actuel</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="5">
+      <formula>AprèsActuel</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="7">
+      <formula>I$8=période_sélectionnée</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="11">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="12">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:BP34">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8:BP8">
+    <cfRule type="expression" dxfId="0" priority="8">
+      <formula>I$8=période_sélectionnée</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="42" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1786,6 +1997,11 @@
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>